<commit_message>
updating figures and excel figures
</commit_message>
<xml_diff>
--- a/international procurement.xlsx
+++ b/international procurement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bomprezzi\Python\UST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pietr\Python\UST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED33E834-5A98-4735-94BA-9BFF299CC44B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14D5EB0-5DAF-4D0B-A4CC-A9C7EE4DBFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11025" xr2:uid="{0529AE6F-DC04-4055-8F86-0EFFF249CC72}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0529AE6F-DC04-4055-8F86-0EFFF249CC72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,36 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="49">
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>Denmark</t>
-  </si>
-  <si>
-    <t>Iceland</t>
-  </si>
-  <si>
-    <t>Lithuania</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="48">
   <si>
     <t>euro</t>
   </si>
@@ -63,39 +50,12 @@
     <t>international initiative</t>
   </si>
   <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Croatia</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>Luxembourg</t>
-  </si>
-  <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
-    <t>Romania</t>
-  </si>
-  <si>
     <t>NATO CAP</t>
   </si>
   <si>
     <t>NORDEFCO</t>
   </si>
   <si>
-    <t>Finland</t>
-  </si>
-  <si>
     <t>EPF</t>
   </si>
   <si>
@@ -108,70 +68,118 @@
     <t>T-72EA</t>
   </si>
   <si>
-    <t>Czechia</t>
-  </si>
-  <si>
     <t>item</t>
   </si>
   <si>
     <t>F-16</t>
   </si>
   <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>Bulgaria</t>
-  </si>
-  <si>
-    <t>Cyprus</t>
-  </si>
-  <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
-    <t>Estonia</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>Hungary</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Latvia</t>
-  </si>
-  <si>
-    <t>Malta</t>
-  </si>
-  <si>
-    <t>Poland</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Slovakia</t>
-  </si>
-  <si>
-    <t>Slovenia</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
     <t>Tank coalition*</t>
   </si>
   <si>
     <t>Aviation coalition*</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>NZ</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>ES</t>
   </si>
 </sst>
 </file>
@@ -224,7 +232,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{831BCCFC-DA6F-45AE-81C0-E6D93AD67D61}"/>
@@ -542,39 +550,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD03644-D37E-4753-96A7-4E89258E1F3A}">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>22799502.556307863</v>
@@ -583,12 +591,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>49595195.968044609</v>
@@ -597,12 +605,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>3603412.9692832762</v>
@@ -611,12 +619,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>6000000</v>
@@ -625,12 +633,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>100000000</v>
@@ -639,12 +647,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>34398541.501840323</v>
@@ -653,12 +661,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>128994530.63190122</v>
@@ -667,12 +675,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>12020056.322549626</v>
@@ -681,12 +689,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>288025069.7020669</v>
@@ -695,12 +703,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>288025069.7020669</v>
@@ -709,12 +717,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>2840102.2436807724</v>
@@ -723,12 +731,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D13">
         <v>12021398.088597704</v>
@@ -737,12 +745,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D14">
         <v>8000000</v>
@@ -751,12 +759,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D15">
         <v>1500000</v>
@@ -765,12 +773,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D16">
         <v>23904932.983280364</v>
@@ -779,12 +787,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>33715628.022661321</v>
@@ -793,12 +801,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D18">
         <v>500000</v>
@@ -807,12 +815,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D19">
         <v>13404107.018390436</v>
@@ -821,12 +829,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D20">
         <v>40000000</v>
@@ -835,12 +843,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D21">
         <v>1365.1877133105802</v>
@@ -849,12 +857,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D22">
         <v>3556313.9931740616</v>
@@ -863,12 +871,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D23">
         <v>28401022.436807726</v>
@@ -877,12 +885,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D24">
         <v>3400000</v>
@@ -891,12 +899,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D25">
         <v>8000000</v>
@@ -905,12 +913,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D26">
         <v>25000000</v>
@@ -919,12 +927,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D27">
         <v>5916499.2185755745</v>
@@ -933,12 +941,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D28">
         <v>2511721.3663764233</v>
@@ -947,12 +955,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D29">
         <v>1032596.5617325295</v>
@@ -961,12 +969,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D30">
         <v>418620.22772940388</v>
@@ -975,12 +983,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D31">
         <v>284010224.36807722</v>
@@ -989,12 +997,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D32">
         <v>785761.62075168034</v>
@@ -1003,12 +1011,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D33">
         <v>378680.29915743636</v>
@@ -1017,12 +1025,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D34">
         <v>5151452.709664125</v>
@@ -1031,12 +1039,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D35">
         <v>7727179.0644961884</v>
@@ -1045,12 +1053,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
         <v>20</v>
-      </c>
-      <c r="C36" t="s">
-        <v>7</v>
       </c>
       <c r="D36">
         <v>11521002.788082674</v>
@@ -1059,12 +1067,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
         <v>20</v>
-      </c>
-      <c r="C37" t="s">
-        <v>7</v>
       </c>
       <c r="D37">
         <v>69126016.728496045</v>
@@ -1073,12 +1081,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D38">
         <v>20106160.5275857</v>
@@ -1087,12 +1095,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D39" s="1">
         <v>10583932.092428511</v>
@@ -1101,12 +1109,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D40" s="1">
         <v>10583932.092428511</v>
@@ -1115,12 +1123,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D41" s="1">
         <v>10583932.092428511</v>
@@ -1129,12 +1137,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D42">
         <v>157484146.50780189</v>
@@ -1143,12 +1151,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D43">
         <v>193129227.55341485</v>
@@ -1157,12 +1165,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D44">
         <v>24395038.762887333</v>
@@ -1171,12 +1179,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
         <v>23</v>
-      </c>
-      <c r="C45" t="s">
-        <v>14</v>
       </c>
       <c r="D45">
         <v>21476235.15657175</v>
@@ -1185,12 +1193,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D46">
         <v>8634171.9406932537</v>
@@ -1199,12 +1207,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D47">
         <v>86248244.841722324</v>
@@ -1213,12 +1221,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D48">
         <v>134194881.05625987</v>
@@ -1227,12 +1235,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D49">
         <v>11278483.82477692</v>
@@ -1241,12 +1249,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D50">
         <v>100582453.97555456</v>
@@ -1255,12 +1263,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D51">
         <v>971991928.32216668</v>
@@ -1269,12 +1277,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D52">
         <v>1443411850.5035539</v>
@@ -1283,12 +1291,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D53">
         <v>70165326.357216597</v>
@@ -1297,12 +1305,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D54">
         <v>56585432.151435241</v>
@@ -1311,12 +1319,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D55">
         <v>119723685.02737039</v>
@@ -1325,12 +1333,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D56">
         <v>702565986.75444949</v>
@@ -1339,12 +1347,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D57">
         <v>12420911.017303396</v>
@@ -1353,12 +1361,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D58">
         <v>20028134.569839548</v>
@@ -1367,12 +1375,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D59">
         <v>18676229.246147268</v>
@@ -1381,12 +1389,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D60">
         <v>4867125.4718646277</v>
@@ -1395,12 +1403,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D61">
         <v>325344296.73166084</v>
@@ -1409,12 +1417,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D62">
         <v>211278465.41000199</v>
@@ -1423,12 +1431,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D63">
         <v>82016742.119404748</v>
@@ -1437,12 +1445,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D64">
         <v>88644732.146417215</v>
@@ -1451,12 +1459,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D65">
         <v>37723649.442471415</v>
@@ -1465,12 +1473,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D66">
         <v>19455851.711810935</v>
@@ -1479,12 +1487,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D67">
         <v>473278876.07485616</v>
@@ -1493,12 +1501,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D68">
         <v>204397893.3223455</v>
@@ -1507,15 +1515,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D69">
         <v>82500000</v>
@@ -1524,15 +1532,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D70">
         <v>82500000</v>
@@ -1541,15 +1549,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D71">
         <v>739817402.44248784</v>
@@ -1558,15 +1566,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D72">
         <v>739817402.44248784</v>
@@ -1575,15 +1583,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D73">
         <f>22948962.7418097/3</f>
@@ -1593,15 +1601,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C74" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D74">
         <f>22948962.7418097/3</f>
@@ -1611,15 +1619,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D75">
         <f>22948962.7418097/3</f>

</xml_diff>